<commit_message>
data.json file added, containing walk data
</commit_message>
<xml_diff>
--- a/plan/Ideation.xlsx
+++ b/plan/Ideation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JacobField\Desktop\Pawsome Walks\pawsome-walks\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275F2AEE-F867-401F-8A3F-74F2AE40FDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38652DB4-AB90-41EC-9D3C-F3881E814FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="33285" windowHeight="20985" xr2:uid="{7EFFDA69-927E-463F-ADAE-39077247C69D}"/>
+    <workbookView xWindow="28665" yWindow="-135" windowWidth="51870" windowHeight="21150" activeTab="1" xr2:uid="{7EFFDA69-927E-463F-ADAE-39077247C69D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ideation" sheetId="1" r:id="rId1"/>
+    <sheet name="MVP" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Anything:</t>
   </si>
@@ -205,13 +206,43 @@
   </si>
   <si>
     <t>walks table (columns: walkName, walkId, latitude (float), longitude (float), walkLength, (booleans: offLeadArea, woods, fields, river, lake, carPark, scenic, quick, etc), rating…</t>
+  </si>
+  <si>
+    <t>Epics</t>
+  </si>
+  <si>
+    <t>Users Registered:</t>
+  </si>
+  <si>
+    <t>Owner Profiles</t>
+  </si>
+  <si>
+    <t>Dog Profiles</t>
+  </si>
+  <si>
+    <t>MVP: Epics</t>
+  </si>
+  <si>
+    <t>Users Regietered</t>
+  </si>
+  <si>
+    <t>Walk Search</t>
+  </si>
+  <si>
+    <t>Favourites List</t>
+  </si>
+  <si>
+    <t>Walk Comments</t>
+  </si>
+  <si>
+    <t>Walk Pages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,8 +283,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,28 +353,31 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0BFFFD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3300EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -446,49 +488,37 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -501,18 +531,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -524,58 +542,70 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -590,92 +620,173 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,6 +794,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3300EE"/>
+      <color rgb="FF0BFFFD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1011,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EF0B9B-D78A-47B9-A092-06381BEF4EB8}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,381 +1146,468 @@
     <col min="9" max="9" width="36.5546875" style="11" customWidth="1"/>
     <col min="10" max="10" width="16.109375" style="11" customWidth="1"/>
     <col min="11" max="11" width="34.44140625" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="8.77734375" style="11"/>
+    <col min="12" max="18" width="8.77734375" style="11"/>
+    <col min="19" max="19" width="35.77734375" style="11" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="11"/>
+    <col min="21" max="21" width="31.33203125" style="11" customWidth="1"/>
+    <col min="22" max="22" width="10.88671875" style="11" customWidth="1"/>
+    <col min="23" max="23" width="30.33203125" style="11" customWidth="1"/>
+    <col min="24" max="16384" width="8.77734375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="18" t="s">
+    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C2" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
-      <c r="I2" s="32" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="84"/>
+      <c r="I2" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="34"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="37"/>
+      <c r="S2" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="68"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="87"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="36"/>
-    </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="38"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="39"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="70"/>
+    </row>
+    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="93"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="36"/>
-    </row>
-    <row r="5" spans="1:17" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="80"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="82"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="72"/>
+      <c r="U4" s="72"/>
+      <c r="V4" s="72"/>
+      <c r="W4" s="73"/>
+    </row>
+    <row r="5" spans="1:23" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="18"/>
+      <c r="E5" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="90" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="64"/>
-      <c r="K5" s="43" t="s">
+      <c r="J5" s="33"/>
+      <c r="K5" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="46" t="s">
+      <c r="L5" s="20"/>
+      <c r="M5" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="48"/>
-    </row>
-    <row r="6" spans="1:17" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="78"/>
+      <c r="S5" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5" s="49"/>
+      <c r="U5" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" s="51"/>
+      <c r="W5" s="67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="37"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="38"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="51"/>
-    </row>
-    <row r="7" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+      <c r="L6" s="20"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="26"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="50"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="60"/>
+    </row>
+    <row r="7" spans="1:23" ht="72" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="38"/>
+      <c r="J7" s="20"/>
       <c r="K7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="38"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="54"/>
-    </row>
-    <row r="8" spans="1:17" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L7" s="20"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="29"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="51"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="61"/>
+    </row>
+    <row r="8" spans="1:23" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="38"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="38"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="54"/>
-    </row>
-    <row r="9" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="20"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="61"/>
+    </row>
+    <row r="9" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="28"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="28"/>
+      <c r="F9" s="16"/>
       <c r="G9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="38"/>
+      <c r="J9" s="20"/>
       <c r="K9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="44"/>
-      <c r="M9" s="55" t="s">
+      <c r="L9" s="22"/>
+      <c r="M9" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="56"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="57"/>
-    </row>
-    <row r="10" spans="1:17" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="42"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="53"/>
+      <c r="W9" s="62"/>
+    </row>
+    <row r="10" spans="1:23" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="28"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="38"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L10" s="45"/>
-      <c r="M10" s="58" t="s">
+      <c r="L10" s="23"/>
+      <c r="M10" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="60"/>
-    </row>
-    <row r="11" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="45"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="63"/>
+    </row>
+    <row r="11" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="28"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="38"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="38"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="53"/>
-      <c r="Q11" s="54"/>
-    </row>
-    <row r="12" spans="1:17" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="20"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="29"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="51"/>
+      <c r="W11" s="61"/>
+    </row>
+    <row r="12" spans="1:23" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="28"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="5"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="38"/>
+      <c r="J12" s="20"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="54"/>
-    </row>
-    <row r="13" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="20"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="29"/>
+      <c r="S12" s="55"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="61"/>
+    </row>
+    <row r="13" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="28"/>
+      <c r="F13" s="16"/>
       <c r="G13" s="5" t="s">
         <v>28</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="38"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L13" s="45"/>
-      <c r="M13" s="58" t="s">
+      <c r="L13" s="23"/>
+      <c r="M13" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="60"/>
-    </row>
-    <row r="14" spans="1:17" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="45"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="51"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="54"/>
+      <c r="W13" s="63"/>
+    </row>
+    <row r="14" spans="1:23" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="28"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="38"/>
+      <c r="J14" s="20"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="53"/>
-      <c r="P14" s="53"/>
-      <c r="Q14" s="54"/>
-    </row>
-    <row r="15" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L14" s="20"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="29"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="61"/>
+    </row>
+    <row r="15" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="27"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="28"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J15" s="37"/>
+      <c r="J15" s="19"/>
       <c r="K15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L15" s="38"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="53"/>
-      <c r="P15" s="53"/>
-      <c r="Q15" s="54"/>
-    </row>
-    <row r="16" spans="1:17" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L15" s="20"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="29"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="61"/>
+    </row>
+    <row r="16" spans="1:23" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="29"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="9"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="39"/>
+      <c r="J16" s="21"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="62"/>
-      <c r="O16" s="62"/>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="63"/>
-    </row>
-    <row r="21" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M21" s="41"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="32"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="52"/>
+      <c r="U16" s="59"/>
+      <c r="V16" s="52"/>
+      <c r="W16" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="E2:E4"/>
+  <mergeCells count="7">
+    <mergeCell ref="S2:W4"/>
+    <mergeCell ref="C2:G4"/>
     <mergeCell ref="I2:Q4"/>
     <mergeCell ref="M9:Q9"/>
     <mergeCell ref="M10:Q10"/>
@@ -1413,4 +1617,385 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8F2C69-8777-44AC-8E4E-30BC13570EC6}">
+  <dimension ref="A1:W16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.77734375" style="11"/>
+    <col min="3" max="3" width="39.21875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="11"/>
+    <col min="5" max="5" width="38.88671875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="11"/>
+    <col min="7" max="7" width="35" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" style="11"/>
+    <col min="9" max="9" width="36.5546875" style="11" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" style="11" customWidth="1"/>
+    <col min="11" max="11" width="34.44140625" style="11" customWidth="1"/>
+    <col min="12" max="18" width="8.77734375" style="11"/>
+    <col min="19" max="19" width="35.77734375" style="11" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="11"/>
+    <col min="21" max="21" width="31.33203125" style="11" customWidth="1"/>
+    <col min="22" max="22" width="10.88671875" style="11" customWidth="1"/>
+    <col min="23" max="23" width="30.33203125" style="11" customWidth="1"/>
+    <col min="24" max="16384" width="8.77734375" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C2" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="84"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="87"/>
+    </row>
+    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="92"/>
+      <c r="Q4" s="92"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="92"/>
+      <c r="T4" s="92"/>
+      <c r="U4" s="92"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="93"/>
+    </row>
+    <row r="5" spans="1:23" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="94"/>
+      <c r="I5" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="94"/>
+      <c r="K5" s="75" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="94"/>
+      <c r="M5" s="76" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="78"/>
+      <c r="S5" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="T5" s="94"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="67"/>
+    </row>
+    <row r="6" spans="1:23" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="26"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="60"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="29"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="95"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="95"/>
+      <c r="W7" s="61"/>
+    </row>
+    <row r="8" spans="1:23" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="95"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="95"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="95"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="95"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="95"/>
+      <c r="W8" s="61"/>
+    </row>
+    <row r="9" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="95"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="95"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="42"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="95"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="95"/>
+      <c r="W9" s="62"/>
+    </row>
+    <row r="10" spans="1:23" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="95"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="95"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="45"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="95"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="95"/>
+      <c r="W10" s="63"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="95"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="95"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="95"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="29"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="95"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="95"/>
+      <c r="W11" s="61"/>
+    </row>
+    <row r="12" spans="1:23" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="95"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="95"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="29"/>
+      <c r="S12" s="55"/>
+      <c r="T12" s="95"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="95"/>
+      <c r="W12" s="61"/>
+    </row>
+    <row r="13" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="95"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="45"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="95"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="95"/>
+      <c r="W13" s="63"/>
+    </row>
+    <row r="14" spans="1:23" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="95"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="95"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="29"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="95"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="95"/>
+      <c r="W14" s="61"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="29"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="95"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="95"/>
+      <c r="W15" s="61"/>
+    </row>
+    <row r="16" spans="1:23" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="95"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="32"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="95"/>
+      <c r="U16" s="59"/>
+      <c r="V16" s="95"/>
+      <c r="W16" s="64"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="C2:W4"/>
+    <mergeCell ref="H5:H16"/>
+    <mergeCell ref="J5:J16"/>
+    <mergeCell ref="L5:L16"/>
+    <mergeCell ref="T5:T16"/>
+    <mergeCell ref="V5:V16"/>
+    <mergeCell ref="M5:Q5"/>
+    <mergeCell ref="M9:Q9"/>
+    <mergeCell ref="M10:Q10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>